<commit_message>
Refs #18640 : Update with latest templates.
</commit_message>
<xml_diff>
--- a/lib/xls_templates/service_areas/2018/SHOP_SA_BCBS.xlsx
+++ b/lib/xls_templates/service_areas/2018/SHOP_SA_BCBS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28726"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vsonnathi/Projects/ma/enroll/lib/xls_templates/service_areas/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15980" xr2:uid="{31500CC6-F967-3041-B253-7D24DDC5C021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,17 @@
     <definedName name="States">[1]county!$A$1:$BG$1</definedName>
     <definedName name="YesNo">[1]county!$BH$1:$BH$2</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>2018 Service Area v7.0</t>
   </si>
@@ -162,12 +159,6 @@
     <t>Partial County</t>
   </si>
   <si>
-    <t>Service Area Zip Code(s)</t>
-  </si>
-  <si>
-    <t>Partial County Justification Filename</t>
-  </si>
-  <si>
     <r>
       <t>Required:</t>
     </r>
@@ -243,36 +234,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Required if Partial County is "Yes":
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Enter the zip codes in this county that are covered by this Service Area</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Required if Partial County is "Yes":
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Enter the filename of the partial county justification file you are uploading to SERFF or HIOS</t>
-    </r>
-  </si>
-  <si>
     <t>MAS001</t>
   </si>
   <si>
@@ -280,19 +241,16 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#####"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,12 +330,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -399,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -409,27 +361,27 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -438,17 +390,17 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -457,41 +409,19 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -511,12 +441,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -552,25 +476,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -587,275 +496,22 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1866900</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>139700</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Button 1" descr="To validate the workbook, press ctrl + shift + i" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:ea typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Validate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1866900</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>127000</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1026" name="Button 2" descr="To finalize the workbook and output a xml file press ctrl + shift + f" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1026"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:ea typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Finalize</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>190500</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>101600</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>1866900</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1027" name="Button 3" descr="Create Service Area IDs.  ctrl + shift + r" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1027"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="ctr" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Arial"/>
-                  <a:ea typeface="Arial"/>
-                  <a:cs typeface="Arial"/>
-                </a:rPr>
-                <a:t>Create Service Area IDs</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData fPrintsWithSheet="0"/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -865,7 +521,6 @@
       <sheetName val="EnableMacros"/>
       <sheetName val="Service Areas"/>
       <sheetName val="county"/>
-      <sheetName val="SHOP_SA_BCBS"/>
     </sheetNames>
     <definedNames>
       <definedName name="createServiceArea"/>
@@ -1135,7 +790,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1187,9 +841,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1217,14 +871,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1252,6 +923,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1403,270 +1091,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IU13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2EDAF7-BBB9-794F-846C-FC0021AAA3E9}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="38" customWidth="1"/>
-    <col min="4" max="4" width="28" style="38" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="40" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="41" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" style="39" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="39" hidden="1" customWidth="1"/>
-    <col min="9" max="255" width="8.83203125" style="38" hidden="1" customWidth="1"/>
-    <col min="256" max="16384" width="5.83203125" style="38" hidden="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="84" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:5" ht="97" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>42690</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
-      <c r="F8" s="10"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="F9" s="10"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="F10" s="10"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:8" s="22" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="20" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="66" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="B12" s="19" t="s">
         <v>16</v>
       </c>
+      <c r="C12" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" s="22" customFormat="1" ht="33" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="24" t="s">
+    <row r="13" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="B13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="35" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Enter a 5-digit Issuer ID" promptTitle="Required:" prompt="Enter the Issuer ID" sqref="B6">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select County from List" promptTitle="Required if State is No" prompt="Select the County-FIPS from List" sqref="D13" xr:uid="{16A0C73A-61FD-5948-ACBB-948D7A27853F}">
+      <formula1>MA</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid:" error="Select Yes or No from List" promptTitle="Required if State is No:" prompt="Select No if this Service Area covers the Entire county" sqref="E13" xr:uid="{A3DE485E-D802-2A43-B541-B9645051F3CF}">
+      <formula1>YesNo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select from list" promptTitle="Required:" prompt="Select the Service Area ID" sqref="A13" xr:uid="{6556DA61-C859-9F4F-967A-82EAFE3CED6D}">
+      <formula1>Service</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select Yes or No from List" promptTitle="Required:" prompt="Select &quot;Yes&quot; if this Service Area covers the entire state" sqref="C13" xr:uid="{8D688646-9305-B944-A784-483FC5CB0B3A}">
+      <formula1>YesNo</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Enter a 5-digit Issuer ID" promptTitle="Required:" prompt="Enter the Issuer ID" sqref="B6" xr:uid="{0DF27F00-8490-E746-BEF3-74C51973AA3A}">
       <formula1>AND(ISNUMBER($B$6),LEN($B$6)=5)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select State from list" promptTitle="Required:" prompt="Select State from List" sqref="B7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select State from list" promptTitle="Required:" prompt="Select State from List" sqref="B7" xr:uid="{0C959F75-A6D5-5F43-941B-71790E49C3BA}">
       <formula1>States</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select County from List" promptTitle="Required if State is No" prompt="Select the County-FIPS from List" sqref="D13:D65456">
-      <formula1>MA</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If you chose 'Yes' for 'Partial County', then you are required to enter a filename for the justification of why all the zip codes are not included in this service area." sqref="G13:G65456"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid:" error="Select Yes or No from List" promptTitle="Required if State is No:" prompt="Select No if this Service Area covers the Entire county" sqref="E13:E65456">
-      <formula1>YesNo</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select from list" promptTitle="Required:" prompt="Select the Service Area ID" sqref="A13:A65456">
-      <formula1>Service</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Select Yes or No from List" promptTitle="Required:" prompt="Select &quot;Yes&quot; if this Service Area covers the entire state" sqref="C13:C65456">
-      <formula1>YesNo</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="If you chose 'Yes' for Partial County, you are required to enter the inclusive 5-digit zip code list seperated by commas here." sqref="F13:F65456"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Required:" prompt="Enter the Service Area Name" sqref="B13:B65456"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Required:" prompt="Enter the Service Area Name" sqref="B13" xr:uid="{E5DEAE9E-7530-1A41-873C-2A276D3A3E2F}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId3" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Validate" altText="To validate the workbook, press ctrl + shift + i">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1866900</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>139700</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId4" name="Button 2">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Finalize" altText="To finalize the workbook and output a xml file press ctrl + shift + f">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1866900</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>127000</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId5" name="Button 3">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!createServiceArea" altText="Create Service Area IDs.  ctrl + shift + r">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>190500</xdr:colOff>
-                    <xdr:row>7</xdr:row>
-                    <xdr:rowOff>101600</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>1866900</xdr:colOff>
-                    <xdr:row>9</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-          <mc:Fallback/>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>